<commit_message>
Corrección imágenes, esqueleto guión, solicitudes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion07/SolicitudGrafica_CN_06_07_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion07/SolicitudGrafica_CN_06_07_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion07\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -523,9 +528,6 @@
     <t>Horizontal</t>
   </si>
   <si>
-    <t xml:space="preserve">Los ecosistemas </t>
-  </si>
-  <si>
     <t>Componentes abióticos de los ecosistemas</t>
   </si>
   <si>
@@ -544,30 +546,18 @@
     <t>La unidad más pequeña de la vida es la célula</t>
   </si>
   <si>
-    <t>Organismo o individuo. Una anémona</t>
-  </si>
-  <si>
-    <t>Fotografía de una ballena jorobada</t>
-  </si>
-  <si>
     <t>Una población de algas marinas</t>
   </si>
   <si>
     <t>Comunidad en un arrecife de coral</t>
   </si>
   <si>
-    <t>Los seres vivos se relacionan con su entorno</t>
-  </si>
-  <si>
     <t>Relaciones entre organismos por depredación</t>
   </si>
   <si>
     <t>Interacciones entre hormigas y plantas por depredación</t>
   </si>
   <si>
-    <t>Aves compitiendo por el espacio</t>
-  </si>
-  <si>
     <t>La luz en el bosque es un factor abiótico que genera competencia</t>
   </si>
   <si>
@@ -575,16 +565,31 @@
   </si>
   <si>
     <t>Interacciones por mutualismo</t>
+  </si>
+  <si>
+    <t>Una pluma no puede volar por sí sola, pero un pájaro si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La biósfera </t>
+  </si>
+  <si>
+    <t>Las callosidades de las ballenas jorobadas</t>
+  </si>
+  <si>
+    <t>Los seres vivos se relacionan entre si</t>
+  </si>
+  <si>
+    <t>Las aves compiten por un lugar para hacer sus nidos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -727,7 +732,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,6 +776,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1274,7 +1285,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1476,6 +1487,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1663,6 +1692,424 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$20" fmlaRange="$H$4:$H$7" noThreeD="1" sel="4" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$20" fmlaRange="$I$6:$I$14" noThreeD="1" sel="5" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="4" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$20" fmlaRange="$H$4:$H$7" noThreeD="1" sel="4" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$20" fmlaRange="$I$6:$I$14" noThreeD="1" sel="5" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="4" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2028825</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Drop Down 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2019300</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1657350</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Drop Down 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Drop Down 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Drop Down 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2066925</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Drop Down 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2085975</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1724025</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Drop Down 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Drop Down 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1986,15 +2433,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
@@ -2005,14 +2452,14 @@
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="17" customWidth="1"/>
+    <col min="10" max="10" width="75.5" style="17" customWidth="1"/>
     <col min="11" max="11" width="29.625" style="17" customWidth="1"/>
     <col min="12" max="12" width="20.375" style="2" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" customWidth="1"/>
     <col min="14" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2024,49 +2471,49 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="F2" s="77" t="s">
+      <c r="D2" s="91"/>
+      <c r="F2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="78"/>
+      <c r="G2" s="84"/>
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="92">
         <v>6</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="F3" s="79">
+      <c r="D3" s="93"/>
+      <c r="F3" s="85">
         <v>42078</v>
       </c>
-      <c r="G3" s="80"/>
+      <c r="G3" s="86"/>
       <c r="H3" s="46"/>
       <c r="I3" s="46"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="92" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="5"/>
       <c r="F4" s="45" t="s">
         <v>55</v>
@@ -2079,15 +2526,15 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1">
+    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="94" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="89"/>
+      <c r="D5" s="95"/>
       <c r="E5" s="5"/>
       <c r="F5" s="43" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2099,7 +2546,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2112,7 +2559,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="30" t="s">
         <v>40</v>
@@ -2130,18 +2577,18 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="89"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2150,7 +2597,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1">
+    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
@@ -2185,7 +2632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="70" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -2218,12 +2665,12 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>151</v>
+      <c r="J10" s="81" t="s">
+        <v>165</v>
       </c>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="70" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
@@ -2257,11 +2704,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="70" t="str">
         <f t="shared" ref="A12:A18" si="2">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
         <v>IMG03</v>
@@ -2295,17 +2742,17 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K12" s="19"/>
     </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A13" s="70" t="str">
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="str">
         <f t="shared" si="2"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="26">
-        <v>156725546</v>
+      <c r="B13" s="78">
+        <v>173824550</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>147</v>
@@ -2333,11 +2780,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="70" t="str">
         <f t="shared" si="2"/>
         <v>IMG05</v>
@@ -2371,11 +2818,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="70" t="str">
         <f t="shared" si="2"/>
         <v>IMG06</v>
@@ -2409,11 +2856,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:16" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="16" spans="1:16" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="70" t="str">
         <f t="shared" si="2"/>
         <v>IMG07</v>
@@ -2447,17 +2894,17 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="71" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K16" s="75"/>
     </row>
-    <row r="17" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A17" s="70" t="str">
+    <row r="17" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="77" t="str">
         <f t="shared" si="2"/>
         <v>IMG08</v>
       </c>
-      <c r="B17" s="74">
-        <v>90940253</v>
+      <c r="B17" s="79">
+        <v>76125697</v>
       </c>
       <c r="C17" s="74" t="s">
         <v>147</v>
@@ -2484,12 +2931,12 @@
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J17" s="71" t="s">
-        <v>158</v>
+      <c r="J17" s="80" t="s">
+        <v>164</v>
       </c>
       <c r="K17" s="71"/>
     </row>
-    <row r="18" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="18" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="70" t="str">
         <f t="shared" si="2"/>
         <v>IMG09</v>
@@ -2522,12 +2969,12 @@
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J18" s="71" t="s">
-        <v>159</v>
+      <c r="J18" s="80" t="s">
+        <v>166</v>
       </c>
       <c r="K18" s="71"/>
     </row>
-    <row r="19" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="19" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
@@ -2561,17 +3008,17 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="71" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K19" s="75"/>
     </row>
-    <row r="20" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A20" s="70" t="str">
+    <row r="20" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="77" t="str">
         <f t="shared" ref="A20:A35" si="3">IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE(LEFT(A19,3),IF(MID(A19,4,2)+1&lt;10,CONCATENATE("0",MID(A19,4,2)+1),MID(A19,4,2)+1)),"")</f>
         <v>IMG11</v>
       </c>
-      <c r="B20" s="74">
-        <v>251277730</v>
+      <c r="B20" s="79">
+        <v>85040797</v>
       </c>
       <c r="C20" s="74" t="s">
         <v>147</v>
@@ -2599,11 +3046,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="72" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K20" s="71"/>
     </row>
-    <row r="21" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="21" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="70" t="str">
         <f t="shared" si="3"/>
         <v>IMG12</v>
@@ -2636,12 +3083,12 @@
         <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J21" s="71" t="s">
-        <v>162</v>
+      <c r="J21" s="80" t="s">
+        <v>167</v>
       </c>
       <c r="K21" s="71"/>
     </row>
-    <row r="22" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="22" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="str">
         <f t="shared" si="3"/>
         <v>IMG13</v>
@@ -2675,11 +3122,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="73" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K22" s="72"/>
     </row>
-    <row r="23" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="23" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70" t="str">
         <f t="shared" si="3"/>
         <v>IMG14</v>
@@ -2713,11 +3160,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="72" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K23" s="72"/>
     </row>
-    <row r="24" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="24" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="70" t="str">
         <f t="shared" si="3"/>
         <v>IMG15</v>
@@ -2750,12 +3197,12 @@
         <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J24" s="73" t="s">
-        <v>165</v>
+      <c r="J24" s="82" t="s">
+        <v>168</v>
       </c>
       <c r="K24" s="73"/>
     </row>
-    <row r="25" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="25" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="70" t="str">
         <f t="shared" si="3"/>
         <v>IMG16</v>
@@ -2789,11 +3236,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="73" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K25" s="72"/>
     </row>
-    <row r="26" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="26" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="70" t="str">
         <f t="shared" si="3"/>
         <v>IMG17</v>
@@ -2827,11 +3274,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="73" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K26" s="72"/>
     </row>
-    <row r="27" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1">
+    <row r="27" spans="1:11" s="76" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="70" t="str">
         <f t="shared" si="3"/>
         <v>IMG18</v>
@@ -2865,11 +3312,11 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J27" s="72" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K27" s="72"/>
     </row>
-    <row r="28" spans="1:11" s="12" customFormat="1">
+    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2900,7 +3347,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" spans="1:11" s="12" customFormat="1">
+    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2931,7 +3378,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1">
+    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2962,7 +3409,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1">
+    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2993,7 +3440,7 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1">
+    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3024,7 +3471,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1">
+    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3055,7 +3502,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1">
+    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3086,7 +3533,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1">
+    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3117,7 +3564,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1">
+    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="str">
         <f t="shared" ref="A36:A83" si="5">IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),CONCATENATE(LEFT(A35,3),IF(MID(A35,4,2)+1&lt;10,CONCATENATE("0",MID(A35,4,2)+1),MID(A35,4,2)+1)),"")</f>
         <v/>
@@ -3148,7 +3595,7 @@
       <c r="J36" s="14"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1">
+    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3179,7 +3626,7 @@
       <c r="J37" s="21"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1">
+    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3210,7 +3657,7 @@
       <c r="J38" s="22"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1">
+    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3241,7 +3688,7 @@
       <c r="J39" s="14"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1">
+    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3272,7 +3719,7 @@
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1">
+    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3303,7 +3750,7 @@
       <c r="J41" s="14"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1">
+    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3334,7 +3781,7 @@
       <c r="J42" s="14"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1">
+    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3365,7 +3812,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1">
+    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3396,7 +3843,7 @@
       <c r="J44" s="14"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1">
+    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3427,7 +3874,7 @@
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1">
+    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3458,7 +3905,7 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1">
+    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3489,7 +3936,7 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1">
+    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3520,7 +3967,7 @@
       <c r="J48" s="14"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1">
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3551,7 +3998,7 @@
       <c r="J49" s="14"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1">
+    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3582,7 +4029,7 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1">
+    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3613,7 +4060,7 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1">
+    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3644,7 +4091,7 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1">
+    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3675,7 +4122,7 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1">
+    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3706,7 +4153,7 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1">
+    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3737,7 +4184,7 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1">
+    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3768,7 +4215,7 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1">
+    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3799,7 +4246,7 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1">
+    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3830,7 +4277,7 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1">
+    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3861,7 +4308,7 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1">
+    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3892,7 +4339,7 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1">
+    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3923,7 +4370,7 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1">
+    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3954,7 +4401,7 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1">
+    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3985,7 +4432,7 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1">
+    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4016,7 +4463,7 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1">
+    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4047,7 +4494,7 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1">
+    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4078,7 +4525,7 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1">
+    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4109,7 +4556,7 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1">
+    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4140,7 +4587,7 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1">
+    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4171,7 +4618,7 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1">
+    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4202,7 +4649,7 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1">
+    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4233,7 +4680,7 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1">
+    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4264,7 +4711,7 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1">
+    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4295,7 +4742,7 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1">
+    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4326,7 +4773,7 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1">
+    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4357,7 +4804,7 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1">
+    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4388,7 +4835,7 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1">
+    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4419,7 +4866,7 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1">
+    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4450,7 +4897,7 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1">
+    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4481,7 +4928,7 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1">
+    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4512,7 +4959,7 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1">
+    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4543,7 +4990,7 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1">
+    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4574,7 +5021,7 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1">
+    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -4605,7 +5052,7 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1">
+    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="str">
         <f t="shared" ref="A84:A108" si="9">IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(LEFT(A83,3),IF(MID(A83,4,2)+1&lt;10,CONCATENATE("0",MID(A83,4,2)+1),MID(A83,4,2)+1)),"")</f>
         <v/>
@@ -4636,7 +5083,7 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1">
+    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4667,7 +5114,7 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1">
+    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4698,7 +5145,7 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1">
+    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4729,7 +5176,7 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1">
+    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4760,7 +5207,7 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1">
+    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4791,7 +5238,7 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1">
+    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4822,7 +5269,7 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1">
+    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4853,7 +5300,7 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1">
+    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4884,7 +5331,7 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1">
+    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4915,7 +5362,7 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1">
+    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4946,7 +5393,7 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1">
+    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -4977,7 +5424,7 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1">
+    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5008,7 +5455,7 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1">
+    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5039,7 +5486,7 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1">
+    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5070,7 +5517,7 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1">
+    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5101,7 +5548,7 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1">
+    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5132,7 +5579,7 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1">
+    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5163,7 +5610,7 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1">
+    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5194,7 +5641,7 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1">
+    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5225,7 +5672,7 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1">
+    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5256,7 +5703,7 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1">
+    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5287,7 +5734,7 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1">
+    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5318,7 +5765,7 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1">
+    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5349,7 +5796,7 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1">
+    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -5438,7 +5885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
@@ -5446,7 +5893,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.25" style="28" customWidth="1"/>
     <col min="2" max="2" width="11" style="28"/>
@@ -5457,38 +5904,38 @@
     <col min="12" max="16384" width="11" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94"/>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="100"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="37"/>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="103"/>
       <c r="F2" s="38"/>
     </row>
-    <row r="3" spans="1:11" ht="63">
+    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="37"/>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="109"/>
       <c r="F3" s="38"/>
       <c r="H3" s="28" t="s">
         <v>18</v>
@@ -5503,7 +5950,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5">
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>44</v>
       </c>
@@ -5531,7 +5978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>45</v>
       </c>
@@ -5539,11 +5986,11 @@
       <c r="C5" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="104" t="str">
+      <c r="D5" s="110" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="105"/>
+      <c r="E5" s="111"/>
       <c r="F5" s="38"/>
       <c r="H5" s="28" t="s">
         <v>22</v>
@@ -5558,7 +6005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>10</v>
       </c>
@@ -5580,7 +6027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>11</v>
       </c>
@@ -5588,12 +6035,12 @@
       <c r="C7" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="90" t="str">
+      <c r="D7" s="96" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="97"/>
       <c r="H7" s="28" t="s">
         <v>24</v>
       </c>
@@ -5607,7 +6054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25">
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>53</v>
       </c>
@@ -5626,7 +6073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25">
+    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
         <v>12</v>
       </c>
@@ -5645,7 +6092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="40" t="s">
         <v>36</v>
       </c>
@@ -5664,7 +6111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="28" t="s">
         <v>32</v>
       </c>
@@ -5675,7 +6122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I12" s="28" t="s">
         <v>37</v>
       </c>
@@ -5686,15 +6133,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="92" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="100"/>
       <c r="I13" s="28" t="s">
         <v>33</v>
       </c>
@@ -5705,7 +6152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="39"/>
       <c r="B14" s="37"/>
       <c r="C14" s="37"/>
@@ -5722,17 +6169,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="37"/>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="103"/>
       <c r="J15" s="28">
         <v>12</v>
       </c>
@@ -5740,7 +6187,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1">
+    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
         <v>47</v>
       </c>
@@ -5764,7 +6211,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36" t="s">
         <v>44</v>
       </c>
@@ -5772,12 +6219,12 @@
       <c r="C17" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="98" t="str">
+      <c r="D17" s="104" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="106"/>
       <c r="J17" s="28">
         <v>14</v>
       </c>
@@ -5785,7 +6232,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
         <v>48</v>
       </c>
@@ -5793,12 +6240,12 @@
       <c r="C18" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="90" t="str">
+      <c r="D18" s="96" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="90"/>
-      <c r="F18" s="91"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="97"/>
       <c r="J18" s="28">
         <v>15</v>
       </c>
@@ -5806,7 +6253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>10</v>
       </c>
@@ -5825,7 +6272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="40" t="s">
         <v>51</v>
       </c>
@@ -5847,7 +6294,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="28" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -5864,122 +6311,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K22" s="28">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K23" s="28">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K24" s="28">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K25" s="28">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K26" s="28">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K27" s="28">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K28" s="28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K29" s="28">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K30" s="28">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K31" s="28">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K32" s="28">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K33" s="28">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K34" s="28">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K35" s="28">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="28">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K37" s="28">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K38" s="28">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K39" s="28">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K40" s="28">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K41" s="28">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K42" s="28">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K43" s="28">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K44" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K45" s="28" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -5999,12 +6446,173 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId4" name="Drop Down 6">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2028825</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId5" name="Drop Down 7">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2019300</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1657350</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId6" name="Drop Down 8">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId7" name="Drop Down 11">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId8" name="Drop Down 2">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2066925</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId9" name="Drop Down 4">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2085975</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1724025</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId10" name="Drop Down 5">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -6012,7 +6620,7 @@
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="28" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="28" customWidth="1"/>
@@ -6028,42 +6636,42 @@
     <col min="12" max="16384" width="10.875" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="112" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="112"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
       <c r="H2" s="47" t="s">
         <v>65</v>
       </c>
@@ -6074,7 +6682,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="49" customFormat="1">
+    <row r="3" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>69</v>
       </c>
@@ -6098,7 +6706,7 @@
       <c r="I3" s="48"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:11" s="49" customFormat="1">
+    <row r="4" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>57</v>
       </c>
@@ -6126,7 +6734,7 @@
       </c>
       <c r="J4" s="50"/>
     </row>
-    <row r="5" spans="1:11" s="49" customFormat="1">
+    <row r="5" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
         <v>77</v>
       </c>
@@ -6154,7 +6762,7 @@
       </c>
       <c r="J5" s="52"/>
     </row>
-    <row r="6" spans="1:11" s="49" customFormat="1">
+    <row r="6" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
         <v>58</v>
       </c>
@@ -6186,7 +6794,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="49" customFormat="1" ht="25.5">
+    <row r="7" spans="1:11" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
         <v>80</v>
       </c>
@@ -6214,7 +6822,7 @@
       </c>
       <c r="J7" s="50"/>
     </row>
-    <row r="8" spans="1:11" s="49" customFormat="1" ht="25.5">
+    <row r="8" spans="1:11" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>82</v>
       </c>
@@ -6242,7 +6850,7 @@
       </c>
       <c r="J8" s="50"/>
     </row>
-    <row r="9" spans="1:11" s="49" customFormat="1">
+    <row r="9" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>84</v>
       </c>
@@ -6270,7 +6878,7 @@
       </c>
       <c r="J9" s="50"/>
     </row>
-    <row r="10" spans="1:11" s="49" customFormat="1">
+    <row r="10" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>86</v>
       </c>
@@ -6296,7 +6904,7 @@
       </c>
       <c r="J10" s="50"/>
     </row>
-    <row r="11" spans="1:11" s="49" customFormat="1" ht="25.5">
+    <row r="11" spans="1:11" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="50" t="s">
         <v>89</v>
       </c>
@@ -6324,7 +6932,7 @@
       </c>
       <c r="J11" s="50"/>
     </row>
-    <row r="12" spans="1:11" s="49" customFormat="1">
+    <row r="12" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50" t="s">
         <v>91</v>
       </c>
@@ -6352,7 +6960,7 @@
       </c>
       <c r="J12" s="50"/>
     </row>
-    <row r="13" spans="1:11" ht="63">
+    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>93</v>
       </c>
@@ -6379,7 +6987,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
         <v>97</v>
       </c>
@@ -6403,7 +7011,7 @@
       </c>
       <c r="J14" s="53"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5">
+    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>99</v>
       </c>
@@ -6430,7 +7038,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5">
+    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
         <v>103</v>
       </c>
@@ -6459,7 +7067,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5">
+    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>106</v>
       </c>
@@ -6488,12 +7096,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="59" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
         <v>113</v>
       </c>
@@ -6506,7 +7114,7 @@
       <c r="D21" s="61"/>
       <c r="E21" s="61"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
         <v>114</v>
       </c>
@@ -6519,7 +7127,7 @@
       <c r="D22" s="64"/>
       <c r="E22" s="64"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="s">
         <v>115</v>
       </c>
@@ -6532,7 +7140,7 @@
       <c r="D23" s="64"/>
       <c r="E23" s="64"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5">
+    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
         <v>116</v>
       </c>
@@ -6545,7 +7153,7 @@
       <c r="D24" s="64"/>
       <c r="E24" s="64"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="63" t="s">
         <v>117</v>
       </c>
@@ -6558,7 +7166,7 @@
       <c r="D25" s="64"/>
       <c r="E25" s="64"/>
     </row>
-    <row r="26" spans="1:11" ht="63">
+    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="63" t="s">
         <v>118</v>
       </c>

</xml_diff>